<commit_message>
Added new charts with the results of the analysis, where the most effective strains can be seen.
</commit_message>
<xml_diff>
--- a/AnovaGHResults.xlsx
+++ b/AnovaGHResults.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Desktop\PlantHealth Master\Data Analysis\Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Desktop\PlantHealth Master\Data Analysis\Project\Data\DA_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A96C60F-A7FE-4865-A08C-FBC0AA93ACB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174600E0-18C0-4153-89A2-C4FFAD038EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F59DDA7-F2A5-4E5D-BA59-2D43B75CD44F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F59DDA7-F2A5-4E5D-BA59-2D43B75CD44F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results.Bean" sheetId="2" r:id="rId2"/>
+    <sheet name="Results.Soy" sheetId="3" r:id="rId3"/>
+    <sheet name="Results.Maize" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="45">
   <si>
     <t>Plant High</t>
   </si>
@@ -130,13 +133,52 @@
   </si>
   <si>
     <t>Not possible to do ANOVA</t>
+  </si>
+  <si>
+    <t>Most efficent strain</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Kruskal-Wallis</t>
+  </si>
+  <si>
+    <t>Tukey</t>
+  </si>
+  <si>
+    <t>Duncan</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>65</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +210,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -242,6 +290,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -253,7 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -265,6 +430,100 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis6" xfId="5" builtinId="50"/>
@@ -586,18 +845,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113AC555-0311-4DF9-9A0C-1DF60F657C0D}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -629,7 +889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -661,7 +921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
@@ -696,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>13</v>
@@ -729,13 +989,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -770,7 +1030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>13</v>
@@ -802,14 +1062,26 @@
       <c r="K7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -843,8 +1115,14 @@
       <c r="K9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" t="s">
         <v>13</v>
@@ -876,14 +1154,26 @@
       <c r="K10" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -917,8 +1207,14 @@
       <c r="K12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" t="s">
         <v>13</v>
@@ -950,70 +1246,789 @@
       <c r="K13" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CF335D-4FE0-41D7-9B73-A952CE0B23AF}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="36"/>
+      <c r="B1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="37"/>
+    </row>
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="36"/>
+      <c r="B2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="41">
+        <v>183</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="41">
+        <v>24</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="42"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="41">
+        <v>183</v>
+      </c>
+      <c r="I5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41">
+        <v>68</v>
+      </c>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="42"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41">
+        <v>179</v>
+      </c>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="42"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="41">
+        <v>183</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41">
+        <v>68</v>
+      </c>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="42"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41">
+        <v>179</v>
+      </c>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2D8DB1-CC97-4338-912A-3E843A9E8A47}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="21"/>
+      <c r="B1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="22"/>
+    </row>
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="30"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="31"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="34"/>
+      <c r="B7" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806858E5-CFEA-4A40-A746-E94139BA8908}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="21"/>
+      <c r="B1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="22"/>
+    </row>
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="30"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="30"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="35">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="J3:J7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>